<commit_message>
Segunda version del comparador
</commit_message>
<xml_diff>
--- a/Existing_File.xlsx
+++ b/Existing_File.xlsx
@@ -11,15 +11,12 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>sdfas</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Roberto</t>
   </si>
@@ -37,12 +34,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -57,9 +60,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,16 +382,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C6"/>
+  <dimension ref="C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+    <row r="1" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="2">
+        <f>Hoja1!A1</f>
         <v>0</v>
       </c>
     </row>
@@ -408,7 +413,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>